<commit_message>
Local changes on case study.
</commit_message>
<xml_diff>
--- a/EU_output/Lisbon/Processed output.xlsx
+++ b/EU_output/Lisbon/Processed output.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\charl\OneDrive\Documents\ENC_Py3_1\EU_output\Lisbon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a1210607\ENC_Py3_1\EU_output\Lisbon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8A94507722AA4AF68892419574C6C9A9D1E887B1" xr6:coauthVersionLast="21" xr6:coauthVersionMax="21" xr10:uidLastSave="{58CCFF37-C33C-4275-BE4F-054A7036FBA5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7640" activeTab="3" xr2:uid="{580DE663-082E-41A5-B286-BC4717EE6A36}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7635" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Lisbon (c)" sheetId="1" r:id="rId1"/>
@@ -72,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4722,6 +4721,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4796,7 +4796,7 @@
         <c:axId val="582872048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5.000000000000001E-2"/>
+          <c:max val="0.1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4840,6 +4840,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4920,6 +4921,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6744,16 +6746,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>562428</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>77520</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>48</xdr:col>
-      <xdr:colOff>539750</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>54841</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>17318</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7077,16 +7079,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFABFCD1-0EF4-420B-B74F-4C81E1DCA16A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView topLeftCell="A97" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection sqref="A1:F126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7118,7 +7120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7154,7 +7156,7 @@
         <v>2.8011898141986622</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -7190,7 +7192,7 @@
         <v>2.6909746269955903</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -7226,7 +7228,7 @@
         <v>2.5786935158462079</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.1</v>
       </c>
@@ -7262,7 +7264,7 @@
         <v>2.6959732476511817</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7298,7 +7300,7 @@
         <v>2.6152347264270102</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0.1</v>
       </c>
@@ -7334,7 +7336,7 @@
         <v>2.5444951385111447</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.1</v>
       </c>
@@ -7370,7 +7372,7 @@
         <v>2.5875908414109441</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.1</v>
       </c>
@@ -7406,7 +7408,7 @@
         <v>2.381151971606009</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.1</v>
       </c>
@@ -7442,7 +7444,7 @@
         <v>2.4298397527732893</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.1</v>
       </c>
@@ -7478,7 +7480,7 @@
         <v>2.4516601877682467</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.1</v>
       </c>
@@ -7514,7 +7516,7 @@
         <v>2.5337010179614392</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7550,7 +7552,7 @@
         <v>2.5050120108403569</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.1</v>
       </c>
@@ -7586,7 +7588,7 @@
         <v>2.4688500273825205</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.1</v>
       </c>
@@ -7622,7 +7624,7 @@
         <v>2.4711990695825632</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.1</v>
       </c>
@@ -7658,7 +7660,7 @@
         <v>2.415503606297698</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7694,7 +7696,7 @@
         <v>2.5825427055671311</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7730,7 +7732,7 @@
         <v>2.6456109181821734</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>0.1</v>
       </c>
@@ -7766,7 +7768,7 @@
         <v>2.3583861955452212</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7802,7 +7804,7 @@
         <v>2.6354555483281183</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -7838,7 +7840,7 @@
         <v>2.3991195848920226</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>0.05</v>
       </c>
@@ -7874,7 +7876,7 @@
         <v>2.5896909810794897</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.05</v>
       </c>
@@ -7910,7 +7912,7 @@
         <v>2.5671517019000749</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.1</v>
       </c>
@@ -7946,7 +7948,7 @@
         <v>2.4656968669041124</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.1</v>
       </c>
@@ -7982,7 +7984,7 @@
         <v>2.3167272289725971</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8018,7 +8020,7 @@
         <v>2.4913024038104452</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8054,7 +8056,7 @@
         <v>2.441501479540455</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8090,7 +8092,7 @@
         <v>2.5239856723556398</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>0.1</v>
       </c>
@@ -8126,7 +8128,7 @@
         <v>2.4149859489851213</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.05</v>
       </c>
@@ -8162,7 +8164,7 @@
         <v>2.6319914098697352</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8198,7 +8200,7 @@
         <v>2.5002348235320411</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.1</v>
       </c>
@@ -8234,7 +8236,7 @@
         <v>2.3263630851323276</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.1</v>
       </c>
@@ -8270,7 +8272,7 @@
         <v>2.4649420720683959</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8306,7 +8308,7 @@
         <v>2.5242469985674107</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8342,7 +8344,7 @@
         <v>2.3623079800499225</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8378,7 +8380,7 @@
         <v>2.4252348488577722</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>0.1</v>
       </c>
@@ -8414,7 +8416,7 @@
         <v>2.5371519479019788</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.1</v>
       </c>
@@ -8450,7 +8452,7 @@
         <v>2.3194233988991231</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8486,7 +8488,7 @@
         <v>2.3905363428427169</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>0.05</v>
       </c>
@@ -8522,7 +8524,7 @@
         <v>2.410173399390279</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8558,7 +8560,7 @@
         <v>2.3382950949231569</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.1</v>
       </c>
@@ -8594,7 +8596,7 @@
         <v>2.4739673053314446</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.1</v>
       </c>
@@ -8630,7 +8632,7 @@
         <v>2.2291215560036655</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8666,7 +8668,7 @@
         <v>2.4074097615556451</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>0.05</v>
       </c>
@@ -8702,7 +8704,7 @@
         <v>2.3938871180544368</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.05</v>
       </c>
@@ -8738,7 +8740,7 @@
         <v>2.4427295175074661</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8774,7 +8776,7 @@
         <v>2.4773292172491481</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>0.1</v>
       </c>
@@ -8810,7 +8812,7 @@
         <v>2.1971220669710827</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -8846,7 +8848,7 @@
         <v>2.2518897746758242</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.1</v>
       </c>
@@ -8882,7 +8884,7 @@
         <v>2.448357521833155</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.05</v>
       </c>
@@ -8918,7 +8920,7 @@
         <v>2.4127791407034818</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0.05</v>
       </c>
@@ -8954,7 +8956,7 @@
         <v>2.2629809023177283</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.05</v>
       </c>
@@ -8990,7 +8992,7 @@
         <v>2.4543605958107673</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0.1</v>
       </c>
@@ -9026,7 +9028,7 @@
         <v>1.9734087328058596</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -9062,7 +9064,7 @@
         <v>2.0086900536682806</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>0.05</v>
       </c>
@@ -9098,7 +9100,7 @@
         <v>2.3112061677008664</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.05</v>
       </c>
@@ -9134,7 +9136,7 @@
         <v>2.0615434221946431</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -9170,7 +9172,7 @@
         <v>2.4644302694196951</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -9206,7 +9208,7 @@
         <v>2.406818480819513</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9242,7 +9244,7 @@
         <v>2.4403391013739113</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>0.05</v>
       </c>
@@ -9278,7 +9280,7 @@
         <v>2.4737721258528853</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -9314,7 +9316,7 @@
         <v>1.8886208750885154</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>0.05</v>
       </c>
@@ -9350,7 +9352,7 @@
         <v>2.0868227744848706</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.05</v>
       </c>
@@ -9386,7 +9388,7 @@
         <v>2.3515056170817772</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.05</v>
       </c>
@@ -9422,7 +9424,7 @@
         <v>1.9479029955801859</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0.05</v>
       </c>
@@ -9458,7 +9460,7 @@
         <v>2.1497383864841804</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.05</v>
       </c>
@@ -9494,7 +9496,7 @@
         <v>2.2377381696508314</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -9530,7 +9532,7 @@
         <v>2.3305959232481817</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>0.05</v>
       </c>
@@ -9566,7 +9568,7 @@
         <v>2.3377879234896186</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.05</v>
       </c>
@@ -9602,7 +9604,7 @@
         <v>1.7682964623453408</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9638,7 +9640,7 @@
         <v>2.1572272307861153</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9674,7 +9676,7 @@
         <v>1.9321387342584444</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -9710,7 +9712,7 @@
         <v>1.2884130274358894</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9746,7 +9748,7 @@
         <v>2.1639768861950071</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9782,7 +9784,7 @@
         <v>2.3001783632974275</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>0.05</v>
       </c>
@@ -9818,7 +9820,7 @@
         <v>1.251400395241796</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.05</v>
       </c>
@@ -9854,7 +9856,7 @@
         <v>2.2120865677055805</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9890,7 +9892,7 @@
         <v>1.9591889176339246</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -9926,7 +9928,7 @@
         <v>1.7919898369349418</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>0.05</v>
       </c>
@@ -9962,7 +9964,7 @@
         <v>1.1417264254393749</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.05</v>
       </c>
@@ -9998,7 +10000,7 @@
         <v>2.2359430619858465</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10034,7 +10036,7 @@
         <v>2.1733508888116466</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10070,7 +10072,7 @@
         <v>1.6612725026420063</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10106,7 +10108,7 @@
         <v>1.8328330322855191</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10142,7 +10144,7 @@
         <v>1.2374960525526317</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>0.05</v>
       </c>
@@ -10178,7 +10180,7 @@
         <v>2.1426192929688179</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10214,7 +10216,7 @@
         <v>1.8917076387343674</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10250,7 +10252,7 @@
         <v>1.9507306177712906</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10286,7 +10288,7 @@
         <v>2.1788235949710506</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10322,7 +10324,7 @@
         <v>1.6996209410134946</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10358,7 +10360,7 @@
         <v>1.5019533934203593</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>0.05</v>
       </c>
@@ -10394,7 +10396,7 @@
         <v>0.56490146617370174</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10430,7 +10432,7 @@
         <v>1.9660308094107259</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10466,7 +10468,7 @@
         <v>2.1352617766853372</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10502,7 +10504,7 @@
         <v>2.1372675804874395</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10538,7 +10540,7 @@
         <v>2.1134025971471959</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10574,7 +10576,7 @@
         <v>1.1480191883437227</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10610,7 +10612,7 @@
         <v>1.0606851513632214</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10646,7 +10648,7 @@
         <v>0.5010826878693041</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10682,7 +10684,7 @@
         <v>0.50561973270367888</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -10718,7 +10720,7 @@
         <v>0.21895894753035194</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0</v>
       </c>
@@ -10754,7 +10756,7 @@
         <v>1.614704664633714</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0</v>
       </c>
@@ -10790,7 +10792,7 @@
         <v>1.4707472455357014</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0</v>
       </c>
@@ -10826,7 +10828,7 @@
         <v>1.7046654165771971</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0</v>
       </c>
@@ -10862,7 +10864,7 @@
         <v>1.3279376536449881</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0</v>
       </c>
@@ -10898,7 +10900,7 @@
         <v>1.9051632570626986</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0</v>
       </c>
@@ -10934,7 +10936,7 @@
         <v>1.6767163830458616</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0</v>
       </c>
@@ -10970,7 +10972,7 @@
         <v>1.1692855071023625</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0</v>
       </c>
@@ -11006,7 +11008,7 @@
         <v>4.5713384841233731E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0</v>
       </c>
@@ -11042,7 +11044,7 @@
         <v>1.5619365805628931</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0</v>
       </c>
@@ -11078,7 +11080,7 @@
         <v>1.9223145737142553</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0</v>
       </c>
@@ -11114,7 +11116,7 @@
         <v>1.9318230875200695</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0</v>
       </c>
@@ -11150,7 +11152,7 @@
         <v>1.9318230875200695</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0</v>
       </c>
@@ -11186,7 +11188,7 @@
         <v>1.7214275718119012</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0</v>
       </c>
@@ -11222,7 +11224,7 @@
         <v>1.5938782307270383</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0</v>
       </c>
@@ -11258,7 +11260,7 @@
         <v>0.17691391933629386</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0</v>
       </c>
@@ -11294,7 +11296,7 @@
         <v>0.52426505181542482</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0</v>
       </c>
@@ -11330,7 +11332,7 @@
         <v>1.7326642430651198</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0</v>
       </c>
@@ -11366,7 +11368,7 @@
         <v>1.8190722776581172</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0</v>
       </c>
@@ -11402,7 +11404,7 @@
         <v>1.1799054527162904</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0</v>
       </c>
@@ -11438,7 +11440,7 @@
         <v>0.21125586628128395</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0</v>
       </c>
@@ -11474,7 +11476,7 @@
         <v>1.021154033637494</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0</v>
       </c>
@@ -11510,7 +11512,7 @@
         <v>1.1084581194927758</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0</v>
       </c>
@@ -11546,7 +11548,7 @@
         <v>0.56367952805667276</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0</v>
       </c>
@@ -11582,7 +11584,7 @@
         <v>1.8491607715610048</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0</v>
       </c>
@@ -11627,16 +11629,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC056601-D25E-4208-BE28-7FD0BC1BBB9F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView topLeftCell="A107" workbookViewId="0">
       <selection sqref="A1:F126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11668,7 +11670,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.1</v>
       </c>
@@ -11704,7 +11706,7 @@
         <v>1.5368604581362002</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0.1</v>
       </c>
@@ -11740,7 +11742,7 @@
         <v>1.8327049894011702</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9.375E-2</v>
       </c>
@@ -11776,7 +11778,7 @@
         <v>1.6319531175618605</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -11812,7 +11814,7 @@
         <v>1.6479565491816901</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>9.375E-2</v>
       </c>
@@ -11848,7 +11850,7 @@
         <v>1.9554111852609515</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -11884,7 +11886,7 @@
         <v>1.7756202242064036</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.1</v>
       </c>
@@ -11920,7 +11922,7 @@
         <v>1.5584986864478112</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.1</v>
       </c>
@@ -11956,7 +11958,7 @@
         <v>1.2179475078144224</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -11992,7 +11994,7 @@
         <v>2.0134096695078592</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9.375E-2</v>
       </c>
@@ -12028,7 +12030,7 @@
         <v>1.4475129068824242</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.1</v>
       </c>
@@ -12064,7 +12066,7 @@
         <v>1.8781919105194236</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.1</v>
       </c>
@@ -12100,7 +12102,7 @@
         <v>1.2843591061115183</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -12136,7 +12138,7 @@
         <v>1.979178782246922</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -12172,7 +12174,7 @@
         <v>1.7930869604500468</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9.375E-2</v>
       </c>
@@ -12208,7 +12210,7 @@
         <v>1.6908451611381772</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -12244,7 +12246,7 @@
         <v>1.915643054193616</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9.375E-2</v>
       </c>
@@ -12280,7 +12282,7 @@
         <v>1.3242310475156589</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>9.375E-2</v>
       </c>
@@ -12316,7 +12318,7 @@
         <v>1.7615144243554814</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.1</v>
       </c>
@@ -12352,7 +12354,7 @@
         <v>1.6271297042123432</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -12388,7 +12390,7 @@
         <v>1.4698788673960057</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -12424,7 +12426,7 @@
         <v>1.8370885268095913</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.1</v>
       </c>
@@ -12460,7 +12462,7 @@
         <v>1.5546397265820324</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -12496,7 +12498,7 @@
         <v>2.1213965789850082</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -12532,7 +12534,7 @@
         <v>2.0644483514795455</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>9.375E-2</v>
       </c>
@@ -12568,7 +12570,7 @@
         <v>1.9999519753610813</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>0.1</v>
       </c>
@@ -12604,7 +12606,7 @@
         <v>1.243792295996812</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9.375E-2</v>
       </c>
@@ -12640,7 +12642,7 @@
         <v>2.059553282326906</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -12676,7 +12678,7 @@
         <v>1.5970540081111875</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.1</v>
       </c>
@@ -12712,7 +12714,7 @@
         <v>1.8542655876996363</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9.375E-2</v>
       </c>
@@ -12748,7 +12750,7 @@
         <v>1.361868759052649</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>0.1</v>
       </c>
@@ -12784,7 +12786,7 @@
         <v>1.6737068518130052</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9.375E-2</v>
       </c>
@@ -12820,7 +12822,7 @@
         <v>1.7136596739636052</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -12856,7 +12858,7 @@
         <v>2.007104603259382</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>0.1</v>
       </c>
@@ -12892,7 +12894,7 @@
         <v>1.3283621473268803</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -12928,7 +12930,7 @@
         <v>2.2295332112777446</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -12964,7 +12966,7 @@
         <v>1.9383985172144578</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -13000,7 +13002,7 @@
         <v>1.6787151197138273</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -13036,7 +13038,7 @@
         <v>2.1931819712602656</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -13072,7 +13074,7 @@
         <v>1.7567729332226067</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -13108,7 +13110,7 @@
         <v>1.8719685317848436</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>0.1</v>
       </c>
@@ -13144,7 +13146,7 @@
         <v>0.98616788695782209</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -13180,7 +13182,7 @@
         <v>1.4786292434181978</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9.375E-2</v>
       </c>
@@ -13216,7 +13218,7 @@
         <v>1.1200514775808483</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -13252,7 +13254,7 @@
         <v>2.1332651570622376</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.1</v>
       </c>
@@ -13288,7 +13290,7 @@
         <v>1.2823218687426492</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -13324,7 +13326,7 @@
         <v>2.0685272902188903</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -13360,7 +13362,7 @@
         <v>1.6696552670181317</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -13396,7 +13398,7 @@
         <v>1.8460860180751655</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>0.1</v>
       </c>
@@ -13432,7 +13434,7 @@
         <v>1.0841758068995631</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>9.375E-2</v>
       </c>
@@ -13468,7 +13470,7 @@
         <v>1.4226648200295215</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>9.375E-2</v>
       </c>
@@ -13504,7 +13506,7 @@
         <v>1.4324662474766958</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.1</v>
       </c>
@@ -13540,7 +13542,7 @@
         <v>1.4040005492478729</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9.375E-2</v>
       </c>
@@ -13576,7 +13578,7 @@
         <v>1.7854101261804223</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -13612,7 +13614,7 @@
         <v>1.246793957224986</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -13648,7 +13650,7 @@
         <v>1.9991698189835554</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.1</v>
       </c>
@@ -13684,7 +13686,7 @@
         <v>1.5919564334332015</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9.375E-2</v>
       </c>
@@ -13720,7 +13722,7 @@
         <v>1.5509394055598373</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -13756,7 +13758,7 @@
         <v>1.5678259468719209</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9.375E-2</v>
       </c>
@@ -13792,7 +13794,7 @@
         <v>1.1959312256206851</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -13828,7 +13830,7 @@
         <v>2.2682420686567681</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -13864,7 +13866,7 @@
         <v>1.7492842231211259</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -13900,7 +13902,7 @@
         <v>1.7765319197940133</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9.375E-2</v>
       </c>
@@ -13936,7 +13938,7 @@
         <v>1.7061655751830953</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.1</v>
       </c>
@@ -13972,7 +13974,7 @@
         <v>0.83691749204012766</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -14008,7 +14010,7 @@
         <v>2.006122405339644</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -14044,7 +14046,7 @@
         <v>2.217828890183227</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -14080,7 +14082,7 @@
         <v>1.9087856627074558</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9.375E-2</v>
       </c>
@@ -14116,7 +14118,7 @@
         <v>1.3209838705770289</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -14152,7 +14154,7 @@
         <v>1.9493283120785829</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.1</v>
       </c>
@@ -14188,7 +14190,7 @@
         <v>1.1266265195449137</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -14224,7 +14226,7 @@
         <v>1.3339224834290611</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -14260,7 +14262,7 @@
         <v>1.8859880629279164</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>0.1</v>
       </c>
@@ -14296,7 +14298,7 @@
         <v>0.96053833418297718</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9.375E-2</v>
       </c>
@@ -14332,7 +14334,7 @@
         <v>0.97212504462125282</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -14368,7 +14370,7 @@
         <v>1.3472005752997631</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -14404,7 +14406,7 @@
         <v>1.5611355039952644</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -14440,7 +14442,7 @@
         <v>1.6731782747924762</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -14476,7 +14478,7 @@
         <v>1.4784466093270723</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -14512,7 +14514,7 @@
         <v>1.5074706802277882</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -14548,7 +14550,7 @@
         <v>2.119164979690348</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -14584,7 +14586,7 @@
         <v>2.05048798378311</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>0.1</v>
       </c>
@@ -14620,7 +14622,7 @@
         <v>1.2977224920339587</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -14656,7 +14658,7 @@
         <v>1.1052114551615153</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -14692,7 +14694,7 @@
         <v>1.659448905305495</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>9.375E-2</v>
       </c>
@@ -14728,7 +14730,7 @@
         <v>1.0686889292360626</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -14764,7 +14766,7 @@
         <v>1.6209635290215938</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -14800,7 +14802,7 @@
         <v>1.2409666516473852</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>0.1</v>
       </c>
@@ -14836,7 +14838,7 @@
         <v>0.75172520822446309</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>9.375E-2</v>
       </c>
@@ -14872,7 +14874,7 @@
         <v>1.4427223215397902</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -14908,7 +14910,7 @@
         <v>1.4284058853215382</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -14944,7 +14946,7 @@
         <v>2.0530744611746012</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -14980,7 +14982,7 @@
         <v>1.2369811035357805</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>9.375E-2</v>
       </c>
@@ -15016,7 +15018,7 @@
         <v>0.88645183061176569</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15052,7 +15054,7 @@
         <v>2.2341324383430927</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15088,7 +15090,7 @@
         <v>1.8133535394605271</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -15124,7 +15126,7 @@
         <v>1.7724188306482382</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -15160,7 +15162,7 @@
         <v>1.9833170729029028</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15196,7 +15198,7 @@
         <v>1.5786360637702308</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -15232,7 +15234,7 @@
         <v>1.045350390237108</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15268,7 +15270,7 @@
         <v>2.2722558878740076</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -15304,7 +15306,7 @@
         <v>1.2181000846239938</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15340,7 +15342,7 @@
         <v>1.4111477385980031</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -15376,7 +15378,7 @@
         <v>1.5922376360352866</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -15412,7 +15414,7 @@
         <v>1.7885941356995545</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0.1</v>
       </c>
@@ -15448,7 +15450,7 @@
         <v>1.5551509421653114</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15484,7 +15486,7 @@
         <v>2.1300241967065836</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15520,7 +15522,7 @@
         <v>1.7358301380336321</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15556,7 +15558,7 @@
         <v>1.9561323131541699</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>9.375E-2</v>
       </c>
@@ -15592,7 +15594,7 @@
         <v>1.7102479292679964</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15628,7 +15630,7 @@
         <v>2.0967811898581585</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0.1</v>
       </c>
@@ -15664,7 +15666,7 @@
         <v>1.3481714989051095</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15700,7 +15702,7 @@
         <v>1.8875733976805225</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -15736,7 +15738,7 @@
         <v>1.3304790389673673</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>9.375E-2</v>
       </c>
@@ -15772,7 +15774,7 @@
         <v>1.5009841486725048</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -15808,7 +15810,7 @@
         <v>1.837093553479628</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -15844,7 +15846,7 @@
         <v>1.6439726188635184</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0.1</v>
       </c>
@@ -15880,7 +15882,7 @@
         <v>1.441186692382699</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>9.375E-2</v>
       </c>
@@ -15916,7 +15918,7 @@
         <v>1.5542513276543306</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -15952,7 +15954,7 @@
         <v>1.7504807450998059</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -15988,7 +15990,7 @@
         <v>1.8491454290561105</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16024,7 +16026,7 @@
         <v>1.6541006164277356</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -16060,7 +16062,7 @@
         <v>1.9750929757857436</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -16096,7 +16098,7 @@
         <v>1.8083268804702448</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>8.1250000000000003E-2</v>
       </c>
@@ -16132,7 +16134,7 @@
         <v>1.7201050140999894</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -16178,16 +16180,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E2F89D-AE8F-4001-9C47-A0CE1366F7A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:F126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -16219,7 +16221,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16255,7 +16257,7 @@
         <v>1.8661416351255584</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16291,7 +16293,7 @@
         <v>1.957817591062333</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16327,7 +16329,7 @@
         <v>2.0347832016710576</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16363,7 +16365,7 @@
         <v>2.1507025365575281</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16399,7 +16401,7 @@
         <v>2.2631849717874672</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16435,7 +16437,7 @@
         <v>1.782637666465706</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16471,7 +16473,7 @@
         <v>1.8895098269612192</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16507,7 +16509,7 @@
         <v>2.0013282348586694</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16543,7 +16545,7 @@
         <v>2.1321062894757121</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16579,7 +16581,7 @@
         <v>2.199661465510546</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16615,7 +16617,7 @@
         <v>1.6495355287648072</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16651,7 +16653,7 @@
         <v>1.8327658117917247</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16687,7 +16689,7 @@
         <v>1.9708418321329382</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16723,7 +16725,7 @@
         <v>2.0859559100163461</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16759,7 +16761,7 @@
         <v>2.2155852027687497</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16795,7 +16797,7 @@
         <v>1.6293342562801314</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16831,7 +16833,7 @@
         <v>1.7691716488780562</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16867,7 +16869,7 @@
         <v>1.8716038833250237</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16903,7 +16905,7 @@
         <v>1.9572607855499831</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16939,7 +16941,7 @@
         <v>2.0079569290760935</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -16975,7 +16977,7 @@
         <v>1.6403354839386599</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -17011,7 +17013,7 @@
         <v>1.7275352034906355</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -17047,7 +17049,7 @@
         <v>1.7730054206681085</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -17083,7 +17085,7 @@
         <v>1.7864578491962502</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8.7499999999999994E-2</v>
       </c>
@@ -17119,7 +17121,7 @@
         <v>1.7188974017518541</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17155,7 +17157,7 @@
         <v>1.7588147458053118</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17191,7 +17193,7 @@
         <v>1.8013814032436866</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17227,7 +17229,7 @@
         <v>1.8418821916965062</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17263,7 +17265,7 @@
         <v>1.9714245689373648</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17299,7 +17301,7 @@
         <v>2.0082760229559482</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17335,7 +17337,7 @@
         <v>1.5690550627903104</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17371,7 +17373,7 @@
         <v>1.6990611661654109</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17407,7 +17409,7 @@
         <v>1.7782005579943159</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17443,7 +17445,7 @@
         <v>1.920613993722986</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17479,7 +17481,7 @@
         <v>2.0150206279529073</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17515,7 +17517,7 @@
         <v>1.4849053941373334</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17551,7 +17553,7 @@
         <v>1.5723001467942406</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17587,7 +17589,7 @@
         <v>1.713856037356523</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17623,7 +17625,7 @@
         <v>1.8484321303836619</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17659,7 +17661,7 @@
         <v>1.9718107502742179</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17695,7 +17697,7 @@
         <v>1.45552450356767</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17731,7 +17733,7 @@
         <v>1.6175543871916154</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17767,7 +17769,7 @@
         <v>1.6933973609077171</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17803,7 +17805,7 @@
         <v>1.728265139275257</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17839,7 +17841,7 @@
         <v>1.7596556815046542</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17875,7 +17877,7 @@
         <v>1.3775609841377465</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17911,7 +17913,7 @@
         <v>1.5255050866587787</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17947,7 +17949,7 @@
         <v>1.5816725012408572</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -17983,7 +17985,7 @@
         <v>1.5929645256670324</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>9.0624999999999997E-2</v>
       </c>
@@ -18019,7 +18021,7 @@
         <v>1.5626697959707914</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>9.375E-2</v>
       </c>
@@ -18055,7 +18057,7 @@
         <v>1.5056565225785399</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>9.375E-2</v>
       </c>
@@ -18091,7 +18093,7 @@
         <v>1.5425945903828899</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>9.375E-2</v>
       </c>
@@ -18127,7 +18129,7 @@
         <v>1.6953559713668698</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>9.375E-2</v>
       </c>
@@ -18163,7 +18165,7 @@
         <v>1.7440562410374065</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>9.375E-2</v>
       </c>
@@ -18199,7 +18201,7 @@
         <v>1.8043232169966696</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>9.375E-2</v>
       </c>
@@ -18235,7 +18237,7 @@
         <v>1.3638539814260833</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>9.375E-2</v>
       </c>
@@ -18271,7 +18273,7 @@
         <v>1.4537255927541937</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>9.375E-2</v>
       </c>
@@ -18307,7 +18309,7 @@
         <v>1.5547525538260616</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>9.375E-2</v>
       </c>
@@ -18343,7 +18345,7 @@
         <v>1.6787203508514283</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>9.375E-2</v>
       </c>
@@ -18379,7 +18381,7 @@
         <v>1.8591223221534254</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>9.375E-2</v>
       </c>
@@ -18415,7 +18417,7 @@
         <v>1.2805402237691137</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>9.375E-2</v>
       </c>
@@ -18451,7 +18453,7 @@
         <v>1.4174743949607285</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>9.375E-2</v>
       </c>
@@ -18487,7 +18489,7 @@
         <v>1.5197092562561241</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>9.375E-2</v>
       </c>
@@ -18523,7 +18525,7 @@
         <v>1.6796606149653761</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>9.375E-2</v>
       </c>
@@ -18559,7 +18561,7 @@
         <v>1.743203035238843</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>9.375E-2</v>
       </c>
@@ -18595,7 +18597,7 @@
         <v>1.2593073977180385</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>9.375E-2</v>
       </c>
@@ -18631,7 +18633,7 @@
         <v>1.3860666131987405</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>9.375E-2</v>
       </c>
@@ -18667,7 +18669,7 @@
         <v>1.4894925474285619</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>9.375E-2</v>
       </c>
@@ -18703,7 +18705,7 @@
         <v>1.5022313099791464</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>9.375E-2</v>
       </c>
@@ -18739,7 +18741,7 @@
         <v>1.5428444361813194</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>9.375E-2</v>
       </c>
@@ -18775,7 +18777,7 @@
         <v>1.1252639678953669</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>9.375E-2</v>
       </c>
@@ -18811,7 +18813,7 @@
         <v>1.2796106639189662</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>9.375E-2</v>
       </c>
@@ -18847,7 +18849,7 @@
         <v>1.3441008953816151</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>9.375E-2</v>
       </c>
@@ -18883,7 +18885,7 @@
         <v>1.4308790677732792</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>9.375E-2</v>
       </c>
@@ -18919,7 +18921,7 @@
         <v>1.380077943867001</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -18955,7 +18957,7 @@
         <v>1.2939605499473317</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -18991,7 +18993,7 @@
         <v>1.3164313141030675</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19027,7 +19029,7 @@
         <v>1.4558472489822223</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19063,7 +19065,7 @@
         <v>1.498498179657703</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19099,7 +19101,7 @@
         <v>1.5940627075342404</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19135,7 +19137,7 @@
         <v>1.1732409923448235</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19171,7 +19173,7 @@
         <v>1.2491558267926401</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19207,7 +19209,7 @@
         <v>1.3261928869401509</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19243,7 +19245,7 @@
         <v>1.5168399821713174</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19279,7 +19281,7 @@
         <v>1.6257868278782408</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19315,7 +19317,7 @@
         <v>1.1338903841811763</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19351,7 +19353,7 @@
         <v>1.2518896460671607</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19387,7 +19389,7 @@
         <v>1.3836924247115636</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19423,7 +19425,7 @@
         <v>1.4475499746804803</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19459,7 +19461,7 @@
         <v>1.5294233873677066</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19495,7 +19497,7 @@
         <v>0.99848839462034</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19531,7 +19533,7 @@
         <v>1.1617557280247959</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19567,7 +19569,7 @@
         <v>1.2484956860957015</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19603,7 +19605,7 @@
         <v>1.3028996497811114</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19639,7 +19641,7 @@
         <v>1.4245053966702141</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19675,7 +19677,7 @@
         <v>0.96676870871531539</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19711,7 +19713,7 @@
         <v>1.0586914746766036</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19747,7 +19749,7 @@
         <v>1.149132041093204</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19783,7 +19785,7 @@
         <v>1.2297337880037591</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>9.6875000000000003E-2</v>
       </c>
@@ -19819,7 +19821,7 @@
         <v>1.2558281861050842</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>0.1</v>
       </c>
@@ -19855,7 +19857,7 @@
         <v>1.1421368192326766</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0.1</v>
       </c>
@@ -19891,7 +19893,7 @@
         <v>1.1909256186770287</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0.1</v>
       </c>
@@ -19927,7 +19929,7 @@
         <v>1.2846009106692464</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0.1</v>
       </c>
@@ -19963,7 +19965,7 @@
         <v>1.3247715153441806</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0.1</v>
       </c>
@@ -19999,7 +20001,7 @@
         <v>1.5118798753514109</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0.1</v>
       </c>
@@ -20035,7 +20037,7 @@
         <v>0.96821477256997213</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0.1</v>
       </c>
@@ -20071,7 +20073,7 @@
         <v>1.0596901612839025</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0.1</v>
       </c>
@@ -20107,7 +20109,7 @@
         <v>1.1644623557480021</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0.1</v>
       </c>
@@ -20143,7 +20145,7 @@
         <v>1.3220641557744666</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0.1</v>
       </c>
@@ -20179,7 +20181,7 @@
         <v>1.4580854235170122</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0.1</v>
       </c>
@@ -20215,7 +20217,7 @@
         <v>0.92681464217408815</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0.1</v>
       </c>
@@ -20251,7 +20253,7 @@
         <v>1.0558419284645284</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0.1</v>
       </c>
@@ -20287,7 +20289,7 @@
         <v>1.1353261242458739</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0.1</v>
       </c>
@@ -20323,7 +20325,7 @@
         <v>1.2196537037286648</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0.1</v>
       </c>
@@ -20359,7 +20361,7 @@
         <v>1.2973623265565812</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0.1</v>
       </c>
@@ -20395,7 +20397,7 @@
         <v>0.84448665839669912</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0.1</v>
       </c>
@@ -20431,7 +20433,7 @@
         <v>1.0021003318839006</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0.1</v>
       </c>
@@ -20467,7 +20469,7 @@
         <v>1.0347723653664658</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0.1</v>
       </c>
@@ -20503,7 +20505,7 @@
         <v>1.2157501133463435</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0.1</v>
       </c>
@@ -20539,7 +20541,7 @@
         <v>1.2854058164073499</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0.1</v>
       </c>
@@ -20575,7 +20577,7 @@
         <v>0.77613100819009606</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0.1</v>
       </c>
@@ -20611,7 +20613,7 @@
         <v>0.93227088847464112</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0.1</v>
       </c>
@@ -20647,7 +20649,7 @@
         <v>0.9755894753986798</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0.1</v>
       </c>
@@ -20683,7 +20685,7 @@
         <v>1.1155663273863055</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0.1</v>
       </c>
@@ -20726,19 +20728,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4B763B-F8A3-45A8-A320-7640A92E28B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AN65" sqref="AN65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="19" max="19" width="8.7265625" customWidth="1"/>
+    <col min="19" max="19" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -20764,7 +20766,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -20820,7 +20822,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -20876,7 +20878,7 @@
         <v>2.93478873613E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0.1</v>
       </c>
@@ -20932,7 +20934,7 @@
         <v>2.8989780675499999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0.1</v>
       </c>
@@ -20988,7 +20990,7 @@
         <v>2.8556102416700001E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0.1</v>
       </c>
@@ -21044,7 +21046,7 @@
         <v>2.8092607582800001E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -21100,7 +21102,7 @@
         <v>2.7530153194500001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0.1</v>
       </c>
@@ -21156,7 +21158,7 @@
         <v>3.0366605767599999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0.1</v>
       </c>
@@ -21212,7 +21214,7 @@
         <v>3.0136102622600001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>0.1</v>
       </c>
@@ -21268,7 +21270,7 @@
         <v>2.9619625620199999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.1</v>
       </c>
@@ -21324,7 +21326,7 @@
         <v>2.9202012720399999E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0.1</v>
       </c>
@@ -21380,7 +21382,7 @@
         <v>2.8736609570800001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>0.1</v>
       </c>
@@ -21436,7 +21438,7 @@
         <v>3.1696872004299999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -21492,7 +21494,7 @@
         <v>3.1359642831700001E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>0.1</v>
       </c>
@@ -21548,7 +21550,7 @@
         <v>3.0771356012200001E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.1</v>
       </c>
@@ -21604,7 +21606,7 @@
         <v>3.0329531952399999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>0.1</v>
       </c>
@@ -21660,7 +21662,7 @@
         <v>2.99875045169E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -21716,7 +21718,7 @@
         <v>3.3019718678999999E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -21772,7 +21774,7 @@
         <v>3.2669903559399999E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>0.1</v>
       </c>
@@ -21828,7 +21830,7 @@
         <v>3.2134686726399998E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -21884,7 +21886,7 @@
         <v>3.1571651859800001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -21940,7 +21942,7 @@
         <v>3.1423392685200002E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>0.05</v>
       </c>
@@ -21996,7 +21998,7 @@
         <v>3.4080104139999998E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>0.05</v>
       </c>
@@ -22052,7 +22054,7 @@
         <v>3.3453981903099998E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>0.1</v>
       </c>
@@ -22108,7 +22110,7 @@
         <v>3.3029109676599999E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>0.1</v>
       </c>
@@ -22164,7 +22166,7 @@
         <v>3.2682524121100003E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -22220,7 +22222,7 @@
         <v>3.2539617490799998E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -22276,7 +22278,7 @@
         <v>3.1074944493099999E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -22332,7 +22334,7 @@
         <v>3.0735440999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>0.1</v>
       </c>
@@ -22388,7 +22390,7 @@
         <v>3.0523488584800001E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>0.05</v>
       </c>
@@ -22444,7 +22446,7 @@
         <v>3.01969357449E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -22500,7 +22502,7 @@
         <v>2.9882176296500002E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>0.1</v>
       </c>
@@ -22556,7 +22558,7 @@
         <v>3.2425664104899998E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>0.1</v>
       </c>
@@ -22612,7 +22614,7 @@
         <v>3.2160277805100002E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -22668,7 +22670,7 @@
         <v>3.1840366341200001E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -22724,7 +22726,7 @@
         <v>3.1342652111100003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -22780,7 +22782,7 @@
         <v>3.0885837933199999E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>0.1</v>
       </c>
@@ -22836,7 +22838,7 @@
         <v>3.3606223866100002E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>0.1</v>
       </c>
@@ -22892,7 +22894,7 @@
         <v>3.3333869579600002E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -22948,7 +22950,7 @@
         <v>3.2872364379500002E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>0.05</v>
       </c>
@@ -23004,7 +23006,7 @@
         <v>3.2514079548299997E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -23060,7 +23062,7 @@
         <v>3.21556146428E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>0.1</v>
       </c>
@@ -23116,7 +23118,7 @@
         <v>3.4935634825100002E-2</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>0.1</v>
       </c>
@@ -23172,7 +23174,7 @@
         <v>3.4417772663400001E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -23228,7 +23230,7 @@
         <v>3.3815965272800001E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>0.05</v>
       </c>
@@ -23284,7 +23286,7 @@
         <v>3.35469349996E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>0.05</v>
       </c>
@@ -23340,7 +23342,7 @@
         <v>3.3143446215199997E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -23396,7 +23398,7 @@
         <v>3.6057816258099999E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>0.1</v>
       </c>
@@ -23452,7 +23454,7 @@
         <v>3.5570470442700002E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -23508,7 +23510,7 @@
         <v>3.5100549054900003E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>0.1</v>
       </c>
@@ -23564,7 +23566,7 @@
         <v>3.46329392587E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>0.05</v>
       </c>
@@ -23620,7 +23622,7 @@
         <v>3.4347207171200003E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>0.05</v>
       </c>
@@ -23676,7 +23678,7 @@
         <v>3.3322002120799998E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>0.05</v>
       </c>
@@ -23732,7 +23734,7 @@
         <v>3.2774190586900002E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>0.1</v>
       </c>
@@ -23788,7 +23790,7 @@
         <v>3.23862230867E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -23844,7 +23846,7 @@
         <v>3.2134082454500001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>0.05</v>
       </c>
@@ -23900,7 +23902,7 @@
         <v>3.1714002684099997E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>0.05</v>
       </c>
@@ -23956,7 +23958,7 @@
         <v>3.4376445304599997E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -24012,7 +24014,7 @@
         <v>3.3974490236500003E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -24068,7 +24070,7 @@
         <v>3.3596929658100003E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -24124,7 +24126,7 @@
         <v>3.30578627234E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>0.05</v>
       </c>
@@ -24180,7 +24182,7 @@
         <v>3.27376428035E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -24236,7 +24238,7 @@
         <v>3.5630397347599999E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>0.05</v>
       </c>
@@ -24292,7 +24294,7 @@
         <v>3.5186718927600003E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>0.05</v>
       </c>
@@ -24348,7 +24350,7 @@
         <v>3.4886207565999999E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>0.05</v>
       </c>
@@ -24404,7 +24406,7 @@
         <v>3.4267741770199998E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>0.05</v>
       </c>
@@ -24460,7 +24462,7 @@
         <v>3.3902199254299999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0.05</v>
       </c>
@@ -24516,7 +24518,7 @@
         <v>3.7099671509099999E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -24572,7 +24574,7 @@
         <v>3.6517502546200002E-2</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>0.05</v>
       </c>
@@ -24628,7 +24630,7 @@
         <v>3.5926007909800002E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>0.05</v>
       </c>
@@ -24684,7 +24686,7 @@
         <v>3.5697987011E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -24740,7 +24742,7 @@
         <v>3.5178204821499998E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -24796,7 +24798,7 @@
         <v>3.7702083784200001E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -24852,7 +24854,7 @@
         <v>3.7171034738500003E-2</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -24908,7 +24910,7 @@
         <v>3.6692307211200002E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -24964,7 +24966,7 @@
         <v>3.6565047074199997E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>0.05</v>
       </c>
@@ -25020,7 +25022,7 @@
         <v>3.6175323713299998E-2</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>0.05</v>
       </c>
@@ -25076,7 +25078,7 @@
         <v>3.5080251789800003E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25132,7 +25134,7 @@
         <v>3.4709727576500003E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25188,7 +25190,7 @@
         <v>3.4291560702500001E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>0.05</v>
       </c>
@@ -25244,7 +25246,7 @@
         <v>3.3924948456799997E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>0.05</v>
       </c>
@@ -25300,7 +25302,7 @@
         <v>3.3473883867499998E-2</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25356,7 +25358,7 @@
         <v>3.6340342401899997E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25412,7 +25414,7 @@
         <v>3.5869177756900003E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25468,7 +25470,7 @@
         <v>3.5527572820700001E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25524,7 +25526,7 @@
         <v>3.49619572196E-2</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>0.05</v>
       </c>
@@ -25580,7 +25582,7 @@
         <v>3.4797429204099999E-2</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25636,7 +25638,7 @@
         <v>3.75968206884E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25692,7 +25694,7 @@
         <v>3.7160543538800002E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25748,7 +25750,7 @@
         <v>3.6842619443199998E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25804,7 +25806,7 @@
         <v>3.6370714519099998E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25860,7 +25862,7 @@
         <v>3.5971301889099999E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>0.05</v>
       </c>
@@ -25916,7 +25918,7 @@
         <v>3.8653501481200003E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -25972,7 +25974,7 @@
         <v>3.8213925537699998E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26028,7 +26030,7 @@
         <v>3.77383510851E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26084,7 +26086,7 @@
         <v>3.7165252846600001E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26140,7 +26142,7 @@
         <v>3.6610563362799997E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26196,7 +26198,7 @@
         <v>3.93685670476E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26252,7 +26254,7 @@
         <v>3.91444528002E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26308,7 +26310,7 @@
         <v>3.8529210191299998E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26364,7 +26366,7 @@
         <v>3.81056324898E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -26420,7 +26422,7 @@
         <v>3.7870000569099997E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>0</v>
       </c>
@@ -26476,7 +26478,7 @@
         <v>3.6740281272999997E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>0</v>
       </c>
@@ -26532,7 +26534,7 @@
         <v>3.6512656311499997E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>0</v>
       </c>
@@ -26588,7 +26590,7 @@
         <v>3.6035737515300002E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>0</v>
       </c>
@@ -26644,7 +26646,7 @@
         <v>3.5636264934400003E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>0</v>
       </c>
@@ -26700,7 +26702,7 @@
         <v>3.5080200877799998E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>0</v>
       </c>
@@ -26756,7 +26758,7 @@
         <v>3.8233604364499997E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>0</v>
       </c>
@@ -26812,7 +26814,7 @@
         <v>3.7816084055399997E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>0</v>
       </c>
@@ -26868,7 +26870,7 @@
         <v>3.7354208078699998E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>0</v>
       </c>
@@ -26924,7 +26926,7 @@
         <v>3.6863999007300002E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>0</v>
       </c>
@@ -26980,7 +26982,7 @@
         <v>3.6556595895600001E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>0</v>
       </c>
@@ -27036,7 +27038,7 @@
         <v>3.9359233450499999E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>0</v>
       </c>
@@ -27092,7 +27094,7 @@
         <v>3.8942894689099998E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>0</v>
       </c>
@@ -27148,7 +27150,7 @@
         <v>3.8589328479300002E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>0</v>
       </c>
@@ -27204,7 +27206,7 @@
         <v>3.81882281283E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>0</v>
       </c>
@@ -27260,7 +27262,7 @@
         <v>3.76864409902E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>0</v>
       </c>
@@ -27316,7 +27318,7 @@
         <v>4.0127076625900003E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>0</v>
       </c>
@@ -27372,7 +27374,7 @@
         <v>3.9678786088400003E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>0</v>
       </c>
@@ -27428,7 +27430,7 @@
         <v>3.94673995609E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>0</v>
       </c>
@@ -27484,7 +27486,7 @@
         <v>3.8895726057E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>0</v>
       </c>
@@ -27540,7 +27542,7 @@
         <v>3.8428189972200003E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>0</v>
       </c>
@@ -27596,7 +27598,7 @@
         <v>4.1109686819500002E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>0</v>
       </c>
@@ -27652,7 +27654,7 @@
         <v>4.0663141405500002E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>0</v>
       </c>
@@ -27708,7 +27710,7 @@
         <v>4.01871968329E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>0</v>
       </c>
@@ -27764,7 +27766,7 @@
         <v>3.9625596752200003E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>0</v>
       </c>

</xml_diff>